<commit_message>
Clocked always block added
</commit_message>
<xml_diff>
--- a/useful references/Operators.xlsx
+++ b/useful references/Operators.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\Specifications\ATE Test Equipment\Harrison Warke\Verilog_HDLBits\useful references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{458F1DA9-B30D-43B8-A789-AF6DD8AF95A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{553B792A-0A44-4A0A-A6EF-F1F9A2C3696A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{01898F28-BC46-43D2-A647-7B9D5792F4BA}"/>
   </bookViews>
@@ -53,9 +53,6 @@
     <t>OR</t>
   </si>
   <si>
-    <t>'</t>
-  </si>
-  <si>
     <t>AND</t>
   </si>
   <si>
@@ -66,6 +63,9 @@
   </si>
   <si>
     <t>~</t>
+  </si>
+  <si>
+    <t>|</t>
   </si>
 </sst>
 </file>
@@ -440,30 +440,30 @@
   <dimension ref="B2:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>

</xml_diff>